<commit_message>
Re-factored the chart classes.
</commit_message>
<xml_diff>
--- a/src/main/resources/Data.xlsx
+++ b/src/main/resources/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -37,18 +37,87 @@
     <t>Cumulative 
 Cases</t>
   </si>
+  <si>
+    <t>Growth formula</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>From day count</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>growth factor</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>how many days after</t>
+  </si>
+  <si>
+    <t>Growth Factor</t>
+  </si>
+  <si>
+    <t>Average GF</t>
+  </si>
+  <si>
+    <t>US G.F</t>
+  </si>
+  <si>
+    <t>x days</t>
+  </si>
+  <si>
+    <t># expected</t>
+  </si>
+  <si>
+    <t>From calc</t>
+  </si>
+  <si>
+    <t>March 13 th Count</t>
+  </si>
+  <si>
+    <r>
+      <t>Y = a  * b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="m/d;@"/>
-    <numFmt numFmtId="168" formatCode="[$-24009]mm/dd/yy;@"/>
-    <numFmt numFmtId="169" formatCode="[$-24009]m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
+    <numFmt numFmtId="165" formatCode="[$-24009]mm/dd/yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-24009]m/d/yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -76,25 +145,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$-24009]mm/dd/yy;@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="m/d;@"/>
+      <numFmt numFmtId="165" formatCode="[$-24009]mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -406,7 +485,7 @@
                   <c:v>69231</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>69709</c:v>
+                  <c:v>85396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -632,7 +711,233 @@
                   <c:v>13885</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>478</c:v>
+                  <c:v>16173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>US!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Growth Factor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>US!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d;@</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>43887</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43888</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43892</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43893</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43895</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43896</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43897</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43899</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43900</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43902</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43903</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43904</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43906</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43907</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43908</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43909</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43910</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43911</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43912</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43913</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43914</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43915</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43916</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>US!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0166666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.098360655737705</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0746268656716418</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3055555555555556</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1914893617021276</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1964285714285714</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2611940298507462</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4201183431952662</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3372093023255813</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2630434782608695</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3029259896729777</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3830911492734479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2340019102196753</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3289473684210527</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3104251601630752</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3235555555555556</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2377434519811954</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2626153011394465</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3117748173614094</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.4201474201474202</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.6254901960784314</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.389484141062939</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3656419160453477</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3116819983546482</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.3150497476979217</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1998352410683315</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.2508763054240595</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.233493666132224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,11 +952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1325853888"/>
-        <c:axId val="1325851712"/>
+        <c:axId val="2064689152"/>
+        <c:axId val="2064689696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1325853888"/>
+        <c:axId val="2064689152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -708,12 +1013,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1325851712"/>
+        <c:crossAx val="2064689696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1325851712"/>
+        <c:axId val="2064689696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +1075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1325853888"/>
+        <c:crossAx val="2064689152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1306,11 +1611,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1325848992"/>
-        <c:axId val="1325852800"/>
+        <c:axId val="2064688608"/>
+        <c:axId val="2064690784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1325848992"/>
+        <c:axId val="2064688608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,12 +1672,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1325852800"/>
+        <c:crossAx val="2064690784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1325852800"/>
+        <c:axId val="2064690784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,7 +1734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1325848992"/>
+        <c:crossAx val="2064688608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2692,14 +2997,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0">
-  <autoFilter ref="A1:C31"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Date" dataDxfId="2">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Cumulative _x000a_Cases"/>
     <tableColumn id="3" name="New Cases"/>
+    <tableColumn id="4" name="Growth Factor" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Cumulative 
+Cases]]/B1</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2709,7 +3018,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C25" totalsRowShown="0">
   <autoFilter ref="A1:C25"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="0">
+    <tableColumn id="1" name="Date" dataDxfId="1">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Cumulative _x000a_Cases"/>
@@ -2982,10 +3291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2993,9 +3302,10 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3005,8 +3315,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43887</v>
       </c>
@@ -3016,8 +3329,13 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="e">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>43888</v>
@@ -3028,10 +3346,15 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B2</f>
+        <v>1.0166666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A33" si="0">A3+1</f>
+        <f t="shared" ref="A4:A31" si="0">A3+1</f>
         <v>43889</v>
       </c>
       <c r="B4">
@@ -3040,8 +3363,13 @@
       <c r="C4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B3</f>
+        <v>1.098360655737705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>43890</v>
@@ -3052,8 +3380,13 @@
       <c r="C5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B4</f>
+        <v>1.0746268656716418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>43891</v>
@@ -3064,8 +3397,13 @@
       <c r="C6">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B5</f>
+        <v>1.3055555555555556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>43892</v>
@@ -3076,8 +3414,13 @@
       <c r="C7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B6</f>
+        <v>1.1914893617021276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>43893</v>
@@ -3088,8 +3431,13 @@
       <c r="C8">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B7</f>
+        <v>1.1964285714285714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>43894</v>
@@ -3100,8 +3448,13 @@
       <c r="C9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B8</f>
+        <v>1.2611940298507462</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>43895</v>
@@ -3112,8 +3465,13 @@
       <c r="C10">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B9</f>
+        <v>1.4201183431952662</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>43896</v>
@@ -3124,8 +3482,13 @@
       <c r="C11">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B10</f>
+        <v>1.4333333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>43897</v>
@@ -3136,8 +3499,13 @@
       <c r="C12">
         <v>116</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B11</f>
+        <v>1.3372093023255813</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>43898</v>
@@ -3148,8 +3516,13 @@
       <c r="C13">
         <v>121</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B12</f>
+        <v>1.2630434782608695</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>43899</v>
@@ -3160,8 +3533,13 @@
       <c r="C14">
         <v>176</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B13</f>
+        <v>1.3029259896729777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>43900</v>
@@ -3172,8 +3550,13 @@
       <c r="C15">
         <v>290</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B14</f>
+        <v>1.3830911492734479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>43901</v>
@@ -3184,8 +3567,13 @@
       <c r="C16">
         <v>245</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B15</f>
+        <v>1.2340019102196753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>43902</v>
@@ -3196,8 +3584,13 @@
       <c r="C17">
         <v>425</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B16</f>
+        <v>1.3289473684210527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>43903</v>
@@ -3208,8 +3601,17 @@
       <c r="C18">
         <v>533</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B17</f>
+        <v>1.3104251601630752</v>
+      </c>
+      <c r="F18">
+        <f>SUM(D3:D18)/17</f>
+        <v>1.1857304553810759</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>43904</v>
@@ -3220,8 +3622,13 @@
       <c r="C19">
         <v>728</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B18</f>
+        <v>1.3235555555555556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>43905</v>
@@ -3232,8 +3639,13 @@
       <c r="C20">
         <v>708</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B19</f>
+        <v>1.2377434519811954</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>43906</v>
@@ -3244,8 +3656,13 @@
       <c r="C21">
         <v>968</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B20</f>
+        <v>1.2626153011394465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>43907</v>
@@ -3256,8 +3673,13 @@
       <c r="C22">
         <v>1451</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B21</f>
+        <v>1.3117748173614094</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>43908</v>
@@ -3268,8 +3690,13 @@
       <c r="C23">
         <v>2265</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B22</f>
+        <v>1.4201474201474202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>43909</v>
@@ -3280,8 +3707,13 @@
       <c r="C24">
         <v>5423</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B23</f>
+        <v>1.6254901960784314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>43910</v>
@@ -3292,8 +3724,13 @@
       <c r="C25">
         <v>5489</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B24</f>
+        <v>1.389484141062939</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>43911</v>
@@ -3304,8 +3741,13 @@
       <c r="C26">
         <v>7160</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B25</f>
+        <v>1.3656419160453477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>43912</v>
@@ -3316,8 +3758,13 @@
       <c r="C27">
         <v>8335</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B26</f>
+        <v>1.3116819983546482</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>43913</v>
@@ -3328,8 +3775,13 @@
       <c r="C28">
         <v>11051</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B27</f>
+        <v>1.3150497476979217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>43914</v>
@@ -3340,8 +3792,13 @@
       <c r="C29">
         <v>9218</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B28</f>
+        <v>1.1998352410683315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>43915</v>
@@ -3352,20 +3809,37 @@
       <c r="C30">
         <v>13885</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B29</f>
+        <v>1.2508763054240595</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>43916</v>
       </c>
       <c r="B31">
-        <v>69709</v>
+        <v>85396</v>
       </c>
       <c r="C31">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16173</v>
+      </c>
+      <c r="D31">
+        <f>Table1[[#This Row],[Cumulative 
+Cases]]/B30</f>
+        <v>1.233493666132224</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31">
+        <f>SUM(D3:D31)/30</f>
+        <v>1.2468269166509072</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -3383,7 +3857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -3696,15 +4170,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D42:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U27" sqref="U27:V27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="42" spans="4:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="D42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="G42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="7"/>
+      <c r="F52">
+        <v>85396</v>
+      </c>
+      <c r="H52">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D53" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53">
+        <v>1.1926830455380999</v>
+      </c>
+      <c r="H53">
+        <v>1.1870000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54">
+        <v>16</v>
+      </c>
+      <c r="H54">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="8">
+        <f>F52* (F53^F54)</f>
+        <v>1431654.6184675505</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57">
+        <f>H52 *(H53^30)</f>
+        <v>86459.54521119225</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="G42:I42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the count for India and US
</commit_message>
<xml_diff>
--- a/src/main/resources/Data.xlsx
+++ b/src/main/resources/Data.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
     <sheet name="India" sheetId="2" r:id="rId2"/>
     <sheet name="Graphs" sheetId="3" r:id="rId3"/>
+    <sheet name="Projection" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -98,17 +99,34 @@
       <t>x</t>
     </r>
   </si>
+  <si>
+    <t>Observed Date:</t>
+  </si>
+  <si>
+    <t>Projected</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Trend</t>
+  </si>
+  <si>
+    <t>Downward</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="[$-24009]mm/dd/yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-24009]m/d/yy;@"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +142,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -141,11 +166,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -154,23 +195,221 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-24009]mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d;@"/>
@@ -952,11 +1191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064689152"/>
-        <c:axId val="2064689696"/>
+        <c:axId val="1192024864"/>
+        <c:axId val="1192023776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064689152"/>
+        <c:axId val="1192024864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,12 +1252,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064689696"/>
+        <c:crossAx val="1192023776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064689696"/>
+        <c:axId val="1192023776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1314,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064689152"/>
+        <c:crossAx val="1192024864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1611,11 +1850,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064688608"/>
-        <c:axId val="2064690784"/>
+        <c:axId val="1192016160"/>
+        <c:axId val="1192019424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064688608"/>
+        <c:axId val="1192016160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,12 +1911,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064690784"/>
+        <c:crossAx val="1192019424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064690784"/>
+        <c:axId val="1192019424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,7 +1973,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064688608"/>
+        <c:crossAx val="1192016160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3000,12 +3239,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0">
   <autoFilter ref="A1:D31"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="2">
+    <tableColumn id="1" name="Date" dataDxfId="21">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Cumulative _x000a_Cases"/>
     <tableColumn id="3" name="New Cases"/>
-    <tableColumn id="4" name="Growth Factor" dataDxfId="0">
+    <tableColumn id="4" name="Growth Factor" dataDxfId="20">
       <calculatedColumnFormula>Table1[[#This Row],[Cumulative 
 Cases]]/B1</calculatedColumnFormula>
     </tableColumn>
@@ -3018,7 +3257,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C25" totalsRowShown="0">
   <autoFilter ref="A1:C25"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataDxfId="1">
+    <tableColumn id="1" name="Date" dataDxfId="19">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Cumulative _x000a_Cases"/>
@@ -3294,7 +3533,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4172,13 +4411,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D42:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4187,11 +4426,11 @@
         <v>3</v>
       </c>
       <c r="E42" s="7"/>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
@@ -4251,7 +4490,7 @@
         <v>14</v>
       </c>
       <c r="F54">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H54">
         <v>30</v>
@@ -4261,9 +4500,9 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="6">
         <f>F52* (F53^F54)</f>
-        <v>1431654.6184675505</v>
+        <v>1006440.6449368802</v>
       </c>
     </row>
     <row r="57" spans="4:8" x14ac:dyDescent="0.25">
@@ -4280,10 +4519,263 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D52:E52"/>
-    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="G42:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>43917</v>
+      </c>
+      <c r="C5" s="12">
+        <v>107994</v>
+      </c>
+      <c r="D5" s="12">
+        <v>104654</v>
+      </c>
+      <c r="E5" s="13">
+        <f>C5-D5</f>
+        <v>3340</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f>B5+1</f>
+        <v>43918</v>
+      </c>
+      <c r="C6" s="12">
+        <v>135542</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <f t="shared" ref="B7:B24" si="0">B6+1</f>
+        <v>43919</v>
+      </c>
+      <c r="C7" s="12">
+        <v>170117</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>43920</v>
+      </c>
+      <c r="C8" s="12">
+        <v>213511</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>43921</v>
+      </c>
+      <c r="C9" s="12">
+        <v>267975</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>43922</v>
+      </c>
+      <c r="C10" s="12">
+        <v>336332</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>43923</v>
+      </c>
+      <c r="C11" s="12">
+        <v>422126</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>43924</v>
+      </c>
+      <c r="C12" s="12">
+        <v>529804</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>43925</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>43926</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>43927</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>43928</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>43929</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>43930</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>43932</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>43933</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>43934</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>43935</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>43936</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1500</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>